<commit_message>
reading from Excel file
</commit_message>
<xml_diff>
--- a/testData/ExelenterEmployees.xlsx
+++ b/testData/ExelenterEmployees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilnoza\Desktop\Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilnoza\Desktop\Programming\TestNGProject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9A4A6C0-11AC-458F-92E7-4B9CB13C461D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3014627F-2B33-4ED5-A4A9-0EA4FB268EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9012" yWindow="1764" windowWidth="13044" windowHeight="10308" xr2:uid="{9F476B80-5E5D-4A24-8BEE-AF3FDC94296B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9F476B80-5E5D-4A24-8BEE-AF3FDC94296B}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
@@ -470,7 +470,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E1" sqref="E1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Retreaving data from excel file using data provider
</commit_message>
<xml_diff>
--- a/testData/ExelenterEmployees.xlsx
+++ b/testData/ExelenterEmployees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilnoza\Desktop\Programming\TestNGProject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D17ADB0-8E9F-4761-BA4B-366A045B9E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA20394-6CB2-47D7-97C1-09A412E212E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9F476B80-5E5D-4A24-8BEE-AF3FDC94296B}"/>
   </bookViews>
@@ -93,19 +93,19 @@
     <t>jess_Shmit@2024</t>
   </si>
   <si>
-    <t>msamuels123</t>
-  </si>
-  <si>
-    <t>sjones12</t>
-  </si>
-  <si>
-    <t>wjohnson123</t>
-  </si>
-  <si>
-    <t>asmith12</t>
-  </si>
-  <si>
-    <t>jshmit123</t>
+    <t>msamuels1235</t>
+  </si>
+  <si>
+    <t>sjones125</t>
+  </si>
+  <si>
+    <t>wjohnson1235</t>
+  </si>
+  <si>
+    <t>asmith125</t>
+  </si>
+  <si>
+    <t>jshmit1235</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>